<commit_message>
Adding all models, creating MCD - MLD and new textures home made
</commit_message>
<xml_diff>
--- a/Documentation/MHG_Journal_de_travail_Tablut.xlsx
+++ b/Documentation/MHG_Journal_de_travail_Tablut.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -32,27 +32,15 @@
     <t>Tâche</t>
   </si>
   <si>
-    <t>Durée (h)</t>
-  </si>
-  <si>
     <t>Commentaires</t>
   </si>
   <si>
-    <t>1h30</t>
-  </si>
-  <si>
-    <t>3h</t>
-  </si>
-  <si>
     <t>Tablut</t>
   </si>
   <si>
     <t>Journal de travail: Herzig Melvyn</t>
   </si>
   <si>
-    <t>Le travail avance plus vite que prévu mais n'est pas achevé.</t>
-  </si>
-  <si>
     <t>Création des scénarii.</t>
   </si>
   <si>
@@ -68,7 +56,40 @@
     <t>Le programme développé portera sur le jeu du "Tablut".</t>
   </si>
   <si>
-    <t>Création des scénarii et maquettes</t>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>Durée</t>
+  </si>
+  <si>
+    <t>1h 30min</t>
+  </si>
+  <si>
+    <t>30min</t>
+  </si>
+  <si>
+    <t>2h 30</t>
+  </si>
+  <si>
+    <t>2h 45min</t>
+  </si>
+  <si>
+    <t>1h 15min</t>
+  </si>
+  <si>
+    <t>15 min</t>
+  </si>
+  <si>
+    <t>Création des use-cases.</t>
+  </si>
+  <si>
+    <t>Création de maquettes.</t>
+  </si>
+  <si>
+    <t>4h</t>
+  </si>
+  <si>
+    <t>Création du MCD - MLD</t>
   </si>
 </sst>
 </file>
@@ -363,7 +384,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -415,6 +436,33 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -432,24 +480,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -731,10 +761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G59"/>
+  <dimension ref="B1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E19" sqref="E19:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -749,7 +779,7 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="25" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="25"/>
@@ -775,7 +805,7 @@
     </row>
     <row r="4" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="26" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C4" s="26"/>
       <c r="D4" s="3"/>
@@ -800,10 +830,10 @@
         <v>1</v>
       </c>
       <c r="D7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="27" t="s">
         <v>2</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>3</v>
       </c>
       <c r="F7" s="27"/>
       <c r="G7" s="27"/>
@@ -813,70 +843,68 @@
         <v>43129</v>
       </c>
       <c r="C8" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="21"/>
+      <c r="E8" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="29"/>
+      <c r="G8" s="30"/>
     </row>
     <row r="9" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B9" s="6">
         <v>43130</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="18"/>
+        <v>10</v>
+      </c>
+      <c r="E9" s="19"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="6">
-        <v>43132</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>10</v>
+        <v>43130</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="17"/>
       <c r="G10" s="18"/>
     </row>
-    <row r="11" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
-        <v>43133</v>
+        <v>43132</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="23"/>
-      <c r="G11" s="24"/>
+        <v>14</v>
+      </c>
+      <c r="E11" s="19"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="21"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
-        <v>43136</v>
+        <v>43132</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="E12" s="16"/>
       <c r="F12" s="17"/>
@@ -884,329 +912,365 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="6">
-        <v>43137</v>
+        <v>43133</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E13" s="16"/>
       <c r="F13" s="17"/>
       <c r="G13" s="18"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="8"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="18"/>
+    <row r="14" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="6">
+        <v>43133</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="31"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="33"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="8"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="18"/>
+      <c r="B15" s="6">
+        <v>43136</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="19"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="21"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="8"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="18"/>
+      <c r="B16" s="6">
+        <v>43137</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="19"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="21"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="8"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="7"/>
+      <c r="B17" s="6">
+        <v>43139</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="E17" s="16"/>
       <c r="F17" s="17"/>
       <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="8"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="18"/>
+      <c r="B18" s="6">
+        <v>43139</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="19"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="21"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="8"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="18"/>
+      <c r="B19" s="6">
+        <v>43139</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="19"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="21"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="8"/>
       <c r="C20" s="14"/>
       <c r="D20" s="7"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="18"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="21"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="8"/>
       <c r="C21" s="14"/>
       <c r="D21" s="7"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="18"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="21"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="8"/>
       <c r="C22" s="14"/>
       <c r="D22" s="7"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="18"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="21"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="8"/>
       <c r="C23" s="14"/>
       <c r="D23" s="7"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="18"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="21"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="8"/>
       <c r="C24" s="14"/>
       <c r="D24" s="7"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="18"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="21"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="8"/>
       <c r="C25" s="14"/>
       <c r="D25" s="7"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="18"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="21"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="8"/>
       <c r="C26" s="14"/>
       <c r="D26" s="7"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="18"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="21"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="8"/>
       <c r="C27" s="14"/>
       <c r="D27" s="7"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="18"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="21"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="8"/>
       <c r="C28" s="14"/>
       <c r="D28" s="7"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="18"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="21"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="8"/>
       <c r="C29" s="14"/>
       <c r="D29" s="7"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="18"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="21"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="8"/>
       <c r="C30" s="14"/>
       <c r="D30" s="7"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="18"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="21"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="8"/>
       <c r="C31" s="14"/>
       <c r="D31" s="7"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="18"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="21"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="8"/>
       <c r="C32" s="14"/>
       <c r="D32" s="7"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="18"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="21"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="8"/>
       <c r="C33" s="14"/>
       <c r="D33" s="7"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="18"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="21"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="8"/>
       <c r="C34" s="14"/>
       <c r="D34" s="7"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="18"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="21"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="8"/>
       <c r="C35" s="14"/>
       <c r="D35" s="7"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="18"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="21"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="8"/>
       <c r="C36" s="14"/>
       <c r="D36" s="7"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="18"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="21"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="8"/>
       <c r="C37" s="14"/>
       <c r="D37" s="7"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="18"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="21"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" s="8"/>
       <c r="C38" s="14"/>
       <c r="D38" s="7"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="18"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="21"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="8"/>
       <c r="C39" s="14"/>
       <c r="D39" s="7"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="18"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="21"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="8"/>
       <c r="C40" s="14"/>
       <c r="D40" s="7"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="18"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="21"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" s="8"/>
       <c r="C41" s="14"/>
       <c r="D41" s="7"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="18"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="21"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" s="8"/>
       <c r="C42" s="14"/>
       <c r="D42" s="7"/>
-      <c r="E42" s="16"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="18"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43" s="8"/>
       <c r="C43" s="14"/>
       <c r="D43" s="7"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="17"/>
-      <c r="G43" s="18"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="21"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" s="8"/>
       <c r="C44" s="14"/>
       <c r="D44" s="7"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="17"/>
-      <c r="G44" s="18"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="21"/>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" s="8"/>
       <c r="C45" s="14"/>
       <c r="D45" s="7"/>
-      <c r="E45" s="16"/>
-      <c r="F45" s="17"/>
-      <c r="G45" s="18"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="21"/>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" s="8"/>
       <c r="C46" s="14"/>
       <c r="D46" s="7"/>
-      <c r="E46" s="16"/>
-      <c r="F46" s="17"/>
-      <c r="G46" s="18"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="21"/>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B47" s="8"/>
       <c r="C47" s="14"/>
       <c r="D47" s="7"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="17"/>
-      <c r="G47" s="18"/>
-    </row>
-    <row r="48" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="9"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="28"/>
-      <c r="F48" s="29"/>
-      <c r="G48" s="30"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="21"/>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B48" s="8"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="21"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="21"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="21"/>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="21"/>
+    </row>
+    <row r="52" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="9"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="22"/>
+      <c r="F52" s="23"/>
+      <c r="G52" s="24"/>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
@@ -1264,23 +1328,63 @@
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
     </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="B1:G2"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E26:G26"/>
     <mergeCell ref="E27:G27"/>
     <mergeCell ref="E28:G28"/>
     <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="E42:G42"/>
     <mergeCell ref="E31:G31"/>
     <mergeCell ref="E32:G32"/>
     <mergeCell ref="E33:G33"/>
@@ -1288,28 +1392,20 @@
     <mergeCell ref="E35:G35"/>
     <mergeCell ref="E36:G36"/>
     <mergeCell ref="E37:G37"/>
-    <mergeCell ref="B1:G2"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Writing intro. and some parts of the analysis
</commit_message>
<xml_diff>
--- a/Documentation/MHG_Journal_de_travail_Tablut.xlsx
+++ b/Documentation/MHG_Journal_de_travail_Tablut.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -90,6 +90,15 @@
   </si>
   <si>
     <t>Création du MCD - MLD</t>
+  </si>
+  <si>
+    <t>Rédaction Introduction/analyse</t>
+  </si>
+  <si>
+    <t>1h30</t>
+  </si>
+  <si>
+    <t>La partie analyse n'est pas encore terminée</t>
   </si>
 </sst>
 </file>
@@ -764,7 +773,7 @@
   <dimension ref="B1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19:G19"/>
+      <selection activeCell="E20" sqref="E20:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1009,10 +1018,18 @@
       <c r="G19" s="21"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="8"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="19"/>
+      <c r="B20" s="6">
+        <v>43140</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>24</v>
+      </c>
       <c r="F20" s="20"/>
       <c r="G20" s="21"/>
     </row>

</xml_diff>

<commit_message>
Adding DB code, beginning UI
</commit_message>
<xml_diff>
--- a/Documentation/MHG_Journal_de_travail_Tablut.xlsx
+++ b/Documentation/MHG_Journal_de_travail_Tablut.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -89,16 +89,31 @@
     <t>4h</t>
   </si>
   <si>
-    <t>Création du MCD - MLD</t>
-  </si>
-  <si>
-    <t>Rédaction Introduction/analyse</t>
-  </si>
-  <si>
     <t>1h30</t>
   </si>
   <si>
     <t>La partie analyse n'est pas encore terminée</t>
+  </si>
+  <si>
+    <t>45 min</t>
+  </si>
+  <si>
+    <t>Création script base de données.</t>
+  </si>
+  <si>
+    <t>Documentation, création de la solution.</t>
+  </si>
+  <si>
+    <t>Rédaction Introduction/analyse.</t>
+  </si>
+  <si>
+    <t>Création du MCD - MLD.</t>
+  </si>
+  <si>
+    <t>Création UI acceuil</t>
+  </si>
+  <si>
+    <t>1h 30 min</t>
   </si>
 </sst>
 </file>
@@ -773,7 +788,7 @@
   <dimension ref="B1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20:G20"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1008,7 +1023,7 @@
         <v>43139</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>10</v>
@@ -1022,37 +1037,55 @@
         <v>43140</v>
       </c>
       <c r="C20" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="19" t="s">
         <v>22</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>24</v>
       </c>
       <c r="F20" s="20"/>
       <c r="G20" s="21"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="8"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="7"/>
+    <row r="21" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B21" s="6">
+        <v>43143</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="E21" s="19"/>
       <c r="F21" s="20"/>
       <c r="G21" s="21"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="8"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="7"/>
+      <c r="B22" s="6">
+        <v>43143</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>23</v>
+      </c>
       <c r="E22" s="19"/>
       <c r="F22" s="20"/>
       <c r="G22" s="21"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="8"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="7"/>
+      <c r="B23" s="6">
+        <v>43144</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>29</v>
+      </c>
       <c r="E23" s="19"/>
       <c r="F23" s="20"/>
       <c r="G23" s="21"/>

</xml_diff>

<commit_message>
Creating UI of profile creation, and implemented the profile creation plus some cues
</commit_message>
<xml_diff>
--- a/Documentation/MHG_Journal_de_travail_Tablut.xlsx
+++ b/Documentation/MHG_Journal_de_travail_Tablut.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -114,6 +114,15 @@
   </si>
   <si>
     <t>1h 30 min</t>
+  </si>
+  <si>
+    <t>Création UI de création de profil, création gestion de profil</t>
+  </si>
+  <si>
+    <t>5h 15min</t>
+  </si>
+  <si>
+    <t>Tout a été implémenté correctement</t>
   </si>
 </sst>
 </file>
@@ -469,6 +478,33 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -477,33 +513,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -788,7 +797,7 @@
   <dimension ref="B1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="E24" sqref="E24:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -802,22 +811,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
     </row>
     <row r="2" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
     </row>
     <row r="3" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
@@ -828,18 +837,18 @@
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="26"/>
+      <c r="C4" s="29"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -856,11 +865,11 @@
       <c r="D7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
     </row>
     <row r="8" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
@@ -872,11 +881,11 @@
       <c r="D8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="29"/>
-      <c r="G8" s="30"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="24"/>
     </row>
     <row r="9" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B9" s="6">
@@ -958,9 +967,9 @@
       <c r="D14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="31"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="33"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="27"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="6">
@@ -1090,11 +1099,19 @@
       <c r="F23" s="20"/>
       <c r="G23" s="21"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="8"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="19"/>
+    <row r="24" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B24" s="6">
+        <v>43146</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>32</v>
+      </c>
       <c r="F24" s="20"/>
       <c r="G24" s="21"/>
     </row>
@@ -1318,9 +1335,9 @@
       <c r="B52" s="9"/>
       <c r="C52" s="15"/>
       <c r="D52" s="10"/>
-      <c r="E52" s="22"/>
-      <c r="F52" s="23"/>
-      <c r="G52" s="24"/>
+      <c r="E52" s="31"/>
+      <c r="F52" s="32"/>
+      <c r="G52" s="33"/>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
@@ -1412,12 +1429,28 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E41:G41"/>
     <mergeCell ref="B1:G2"/>
     <mergeCell ref="B4:C5"/>
     <mergeCell ref="E30:G30"/>
@@ -1434,28 +1467,12 @@
     <mergeCell ref="E29:G29"/>
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding exception to create profile, creating UI managment profile
</commit_message>
<xml_diff>
--- a/Documentation/MHG_Journal_de_travail_Tablut.xlsx
+++ b/Documentation/MHG_Journal_de_travail_Tablut.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -92,9 +92,6 @@
     <t>1h30</t>
   </si>
   <si>
-    <t>La partie analyse n'est pas encore terminée</t>
-  </si>
-  <si>
     <t>45 min</t>
   </si>
   <si>
@@ -122,7 +119,22 @@
     <t>5h 15min</t>
   </si>
   <si>
-    <t>Tout a été implémenté correctement</t>
+    <t>La partie analyse n'est pas encore terminée.</t>
+  </si>
+  <si>
+    <t>Tout a été implémenté correctement sauf la recherche de doublon.</t>
+  </si>
+  <si>
+    <t>30 min</t>
+  </si>
+  <si>
+    <t>Permet de savoir si un profil existe déjà, si la syntax du nom est correct ou si le serveur de base de données est allumé.</t>
+  </si>
+  <si>
+    <t>Création de profil.</t>
+  </si>
+  <si>
+    <t>Création UI gestion de profil.</t>
   </si>
 </sst>
 </file>
@@ -797,7 +809,7 @@
   <dimension ref="B1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24:G24"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1032,7 +1044,7 @@
         <v>43139</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>10</v>
@@ -1046,13 +1058,13 @@
         <v>43140</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>21</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="F20" s="20"/>
       <c r="G20" s="21"/>
@@ -1062,10 +1074,10 @@
         <v>43143</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E21" s="19"/>
       <c r="F21" s="20"/>
@@ -1076,10 +1088,10 @@
         <v>43143</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E22" s="19"/>
       <c r="F22" s="20"/>
@@ -1090,10 +1102,10 @@
         <v>43144</v>
       </c>
       <c r="C23" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>29</v>
       </c>
       <c r="E23" s="19"/>
       <c r="F23" s="20"/>
@@ -1104,29 +1116,43 @@
         <v>43146</v>
       </c>
       <c r="C24" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E24" s="19" t="s">
+      <c r="E24" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="F24" s="20"/>
-      <c r="G24" s="21"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="8"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="21"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="27"/>
+    </row>
+    <row r="25" spans="2:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="6">
+        <v>43147</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" s="26"/>
+      <c r="G25" s="27"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="8"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="7"/>
+      <c r="B26" s="6">
+        <v>43147</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="E26" s="19"/>
       <c r="F26" s="20"/>
       <c r="G26" s="21"/>

</xml_diff>

<commit_message>
Creating disable buttons, adding some logic in the profile managment
</commit_message>
<xml_diff>
--- a/Documentation/MHG_Journal_de_travail_Tablut.xlsx
+++ b/Documentation/MHG_Journal_de_travail_Tablut.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t>Création UI gestion de profil.</t>
+  </si>
+  <si>
+    <t>Logique gestion de profil</t>
+  </si>
+  <si>
+    <t>En cours</t>
   </si>
 </sst>
 </file>
@@ -490,6 +496,33 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -498,33 +531,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -809,7 +815,7 @@
   <dimension ref="B1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="E27" sqref="E27:G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -823,22 +829,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
     </row>
     <row r="3" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
@@ -849,18 +855,18 @@
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="29"/>
+      <c r="C4" s="26"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -893,11 +899,11 @@
       <c r="D8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="23"/>
-      <c r="G8" s="24"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="33"/>
     </row>
     <row r="9" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B9" s="6">
@@ -979,9 +985,9 @@
       <c r="D14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="25"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="29"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="6">
@@ -1121,11 +1127,11 @@
       <c r="D24" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E24" s="25" t="s">
+      <c r="E24" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="F24" s="26"/>
-      <c r="G24" s="27"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="29"/>
     </row>
     <row r="25" spans="2:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="6">
@@ -1137,11 +1143,11 @@
       <c r="D25" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="25" t="s">
+      <c r="E25" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="F25" s="26"/>
-      <c r="G25" s="27"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="29"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="6">
@@ -1158,10 +1164,18 @@
       <c r="G26" s="21"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="8"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="19"/>
+      <c r="B27" s="6">
+        <v>43157</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>38</v>
+      </c>
       <c r="F27" s="20"/>
       <c r="G27" s="21"/>
     </row>
@@ -1361,9 +1375,9 @@
       <c r="B52" s="9"/>
       <c r="C52" s="15"/>
       <c r="D52" s="10"/>
-      <c r="E52" s="31"/>
-      <c r="F52" s="32"/>
-      <c r="G52" s="33"/>
+      <c r="E52" s="22"/>
+      <c r="F52" s="23"/>
+      <c r="G52" s="24"/>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
@@ -1455,28 +1469,12 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
     <mergeCell ref="B1:G2"/>
     <mergeCell ref="B4:C5"/>
     <mergeCell ref="E30:G30"/>
@@ -1493,12 +1491,28 @@
     <mergeCell ref="E29:G29"/>
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Working on getting the stats from the DB for a profile
</commit_message>
<xml_diff>
--- a/Documentation/MHG_Journal_de_travail_Tablut.xlsx
+++ b/Documentation/MHG_Journal_de_travail_Tablut.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -128,9 +128,6 @@
     <t>30 min</t>
   </si>
   <si>
-    <t>Permet de savoir si un profil existe déjà, si la syntax du nom est correct ou si le serveur de base de données est allumé.</t>
-  </si>
-  <si>
     <t>Création de profil.</t>
   </si>
   <si>
@@ -141,6 +138,9 @@
   </si>
   <si>
     <t>En cours</t>
+  </si>
+  <si>
+    <t>Permet de savoir si un profil existe déjà, si la syntaxe du nom est correct ou si le serveur de base de données est allumé.</t>
   </si>
 </sst>
 </file>
@@ -496,6 +496,33 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -504,33 +531,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -814,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27:G27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28:G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -829,22 +829,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
     </row>
     <row r="2" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
     </row>
     <row r="3" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
@@ -855,18 +855,18 @@
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="26"/>
+      <c r="C4" s="29"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -899,11 +899,11 @@
       <c r="D8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="32"/>
-      <c r="G8" s="33"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="24"/>
     </row>
     <row r="9" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B9" s="6">
@@ -985,9 +985,9 @@
       <c r="D14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="27"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="29"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="27"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="6">
@@ -1127,34 +1127,34 @@
       <c r="D24" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E24" s="27" t="s">
+      <c r="E24" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="F24" s="28"/>
-      <c r="G24" s="29"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="27"/>
     </row>
     <row r="25" spans="2:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="6">
         <v>43147</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="F25" s="28"/>
-      <c r="G25" s="29"/>
+      <c r="E25" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="F25" s="26"/>
+      <c r="G25" s="27"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="6">
         <v>43147</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>10</v>
@@ -1168,22 +1168,30 @@
         <v>43157</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>21</v>
       </c>
       <c r="E27" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F27" s="20"/>
       <c r="G27" s="21"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="8"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="19"/>
+      <c r="B28" s="6">
+        <v>43158</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>37</v>
+      </c>
       <c r="F28" s="20"/>
       <c r="G28" s="21"/>
     </row>
@@ -1375,9 +1383,9 @@
       <c r="B52" s="9"/>
       <c r="C52" s="15"/>
       <c r="D52" s="10"/>
-      <c r="E52" s="22"/>
-      <c r="F52" s="23"/>
-      <c r="G52" s="24"/>
+      <c r="E52" s="31"/>
+      <c r="F52" s="32"/>
+      <c r="G52" s="33"/>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
@@ -1469,12 +1477,28 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E41:G41"/>
     <mergeCell ref="B1:G2"/>
     <mergeCell ref="B4:C5"/>
     <mergeCell ref="E30:G30"/>
@@ -1491,28 +1515,12 @@
     <mergeCell ref="E29:G29"/>
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding profile selection UI and fulling the lists with the profiles's name
</commit_message>
<xml_diff>
--- a/Documentation/MHG_Journal_de_travail_Tablut.xlsx
+++ b/Documentation/MHG_Journal_de_travail_Tablut.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
   <si>
     <t>Date</t>
   </si>
@@ -113,9 +113,6 @@
     <t>1h 30 min</t>
   </si>
   <si>
-    <t>Création UI de création de profil, création gestion de profil</t>
-  </si>
-  <si>
     <t>5h 15min</t>
   </si>
   <si>
@@ -134,13 +131,28 @@
     <t>Création UI gestion de profil.</t>
   </si>
   <si>
-    <t>Logique gestion de profil</t>
-  </si>
-  <si>
-    <t>En cours</t>
-  </si>
-  <si>
     <t>Permet de savoir si un profil existe déjà, si la syntaxe du nom est correct ou si le serveur de base de données est allumé.</t>
+  </si>
+  <si>
+    <t>Gestion de profils fonctionnelle avec messages d'erreurs en cas de mauvaise manipulation.</t>
+  </si>
+  <si>
+    <t>En cours.</t>
+  </si>
+  <si>
+    <t>Logique gestion de profil.</t>
+  </si>
+  <si>
+    <t>Création UI de création de profil, création de profil</t>
+  </si>
+  <si>
+    <t>Création UI Sélection des joueurs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logique sélection des joueurs </t>
+  </si>
+  <si>
+    <t>En cours, les drop down list se remplissent. Il faut encore ajouter une erreur si deux même profils sont choisis</t>
   </si>
 </sst>
 </file>
@@ -815,7 +827,7 @@
   <dimension ref="B1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28:G28"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1070,7 +1082,7 @@
         <v>21</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F20" s="20"/>
       <c r="G20" s="21"/>
@@ -1122,13 +1134,13 @@
         <v>43146</v>
       </c>
       <c r="C24" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>30</v>
-      </c>
       <c r="E24" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F24" s="26"/>
       <c r="G24" s="27"/>
@@ -1138,13 +1150,13 @@
         <v>43147</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E25" s="25" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F25" s="26"/>
       <c r="G25" s="27"/>
@@ -1154,7 +1166,7 @@
         <v>43147</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>10</v>
@@ -1168,7 +1180,7 @@
         <v>43157</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>21</v>
@@ -1184,7 +1196,7 @@
         <v>43158</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>21</v>
@@ -1195,29 +1207,51 @@
       <c r="F28" s="20"/>
       <c r="G28" s="21"/>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="8"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="21"/>
+    <row r="29" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="6">
+        <v>43160</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" s="26"/>
+      <c r="G29" s="27"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="8"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="7"/>
+      <c r="B30" s="6">
+        <v>43160</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="E30" s="19"/>
       <c r="F30" s="20"/>
       <c r="G30" s="21"/>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="8"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="21"/>
+    <row r="31" spans="2:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="6">
+        <v>43160</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="F31" s="26"/>
+      <c r="G31" s="27"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="8"/>

</xml_diff>

<commit_message>
Finishing profile selection, adding the board UI and prototype of grid.
</commit_message>
<xml_diff>
--- a/Documentation/MHG_Journal_de_travail_Tablut.xlsx
+++ b/Documentation/MHG_Journal_de_travail_Tablut.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
   <si>
     <t>Date</t>
   </si>
@@ -153,6 +153,18 @@
   </si>
   <si>
     <t>En cours, les drop down list se remplissent. Il faut encore ajouter une erreur si deux même profils sont choisis</t>
+  </si>
+  <si>
+    <t>Fin logique sélection des joueurs</t>
+  </si>
+  <si>
+    <t>Les jouers doivent être sélectionnés pour lancer une partie. Doublon impossible</t>
+  </si>
+  <si>
+    <t>Prototype de remplissage de grille</t>
+  </si>
+  <si>
+    <t>Un table layout panel a été placé au dessous du dessin du plateau, de ce fait il sera possible de placer les pions en fonctions d'une ligne et d'une colonne.</t>
   </si>
 </sst>
 </file>
@@ -447,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -508,6 +520,33 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -517,32 +556,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -827,7 +842,7 @@
   <dimension ref="B1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="E33" sqref="E33:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -911,11 +926,11 @@
       <c r="D8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="23"/>
-      <c r="G8" s="24"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="33"/>
     </row>
     <row r="9" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B9" s="6">
@@ -1253,24 +1268,40 @@
       <c r="F31" s="26"/>
       <c r="G31" s="27"/>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="8"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="21"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="8"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="21"/>
+    <row r="32" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="6">
+        <v>43161</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="F32" s="26"/>
+      <c r="G32" s="27"/>
+    </row>
+    <row r="33" spans="2:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="6">
+        <v>43161</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="F33" s="26"/>
+      <c r="G33" s="27"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="8"/>
+      <c r="B34" s="34"/>
       <c r="C34" s="14"/>
       <c r="D34" s="7"/>
       <c r="E34" s="19"/>
@@ -1417,9 +1448,9 @@
       <c r="B52" s="9"/>
       <c r="C52" s="15"/>
       <c r="D52" s="10"/>
-      <c r="E52" s="31"/>
-      <c r="F52" s="32"/>
-      <c r="G52" s="33"/>
+      <c r="E52" s="22"/>
+      <c r="F52" s="23"/>
+      <c r="G52" s="24"/>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
@@ -1511,28 +1542,12 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
     <mergeCell ref="B1:G2"/>
     <mergeCell ref="B4:C5"/>
     <mergeCell ref="E30:G30"/>
@@ -1549,12 +1564,28 @@
     <mergeCell ref="E29:G29"/>
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding square status, game and player class
</commit_message>
<xml_diff>
--- a/Documentation/MHG_Journal_de_travail_Tablut.xlsx
+++ b/Documentation/MHG_Journal_de_travail_Tablut.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
   <si>
     <t>Date</t>
   </si>
@@ -171,6 +171,12 @@
   </si>
   <si>
     <t>Une classe Square, héritée de picture box a été créée, elle inclut une énumération personnalisée.</t>
+  </si>
+  <si>
+    <t>Ajout des classes "Game" et "Joueur". De plus les cases ont désormais un type.</t>
+  </si>
+  <si>
+    <t>Les type défini si la case est occupée ou non et par qui.</t>
   </si>
 </sst>
 </file>
@@ -517,6 +523,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -526,6 +535,33 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -534,36 +570,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -847,8 +853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34:G34"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38:G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -862,22 +868,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
     </row>
     <row r="3" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
@@ -888,18 +894,18 @@
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="29"/>
+      <c r="C4" s="30"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -916,11 +922,11 @@
       <c r="D7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
     </row>
     <row r="8" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
@@ -932,11 +938,11 @@
       <c r="D8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="23"/>
-      <c r="G8" s="24"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="34"/>
     </row>
     <row r="9" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B9" s="6">
@@ -948,9 +954,9 @@
       <c r="D9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="21"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="22"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="6">
@@ -976,9 +982,9 @@
       <c r="D11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="19"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="21"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="22"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
@@ -1018,9 +1024,9 @@
       <c r="D14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="25"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="27"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="28"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="6">
@@ -1032,9 +1038,9 @@
       <c r="D15" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="19"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="21"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="22"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="6">
@@ -1046,9 +1052,9 @@
       <c r="D16" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="21"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="22"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="6">
@@ -1074,9 +1080,9 @@
       <c r="D18" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="19"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="21"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="22"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="6">
@@ -1088,9 +1094,9 @@
       <c r="D19" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="19"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="21"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="22"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="6">
@@ -1102,11 +1108,11 @@
       <c r="D20" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="F20" s="20"/>
-      <c r="G20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="22"/>
     </row>
     <row r="21" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B21" s="6">
@@ -1118,9 +1124,9 @@
       <c r="D21" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="19"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="21"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="22"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="6">
@@ -1132,9 +1138,9 @@
       <c r="D22" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="19"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="21"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="22"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="6">
@@ -1146,9 +1152,9 @@
       <c r="D23" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="19"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="21"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="22"/>
     </row>
     <row r="24" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B24" s="6">
@@ -1160,11 +1166,11 @@
       <c r="D24" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="25" t="s">
+      <c r="E24" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="F24" s="26"/>
-      <c r="G24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="28"/>
     </row>
     <row r="25" spans="2:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="6">
@@ -1176,11 +1182,11 @@
       <c r="D25" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E25" s="25" t="s">
+      <c r="E25" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="F25" s="26"/>
-      <c r="G25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="28"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="6">
@@ -1192,9 +1198,9 @@
       <c r="D26" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="19"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="21"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="22"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="6">
@@ -1206,11 +1212,11 @@
       <c r="D27" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="19" t="s">
+      <c r="E27" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="20"/>
-      <c r="G27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="22"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="6">
@@ -1222,11 +1228,11 @@
       <c r="D28" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E28" s="19" t="s">
+      <c r="E28" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="F28" s="20"/>
-      <c r="G28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="22"/>
     </row>
     <row r="29" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="6">
@@ -1238,11 +1244,11 @@
       <c r="D29" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="25" t="s">
+      <c r="E29" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="26"/>
-      <c r="G29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="28"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="6">
@@ -1254,9 +1260,9 @@
       <c r="D30" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E30" s="19"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="21"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="22"/>
     </row>
     <row r="31" spans="2:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="6">
@@ -1268,11 +1274,11 @@
       <c r="D31" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="25" t="s">
+      <c r="E31" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="F31" s="26"/>
-      <c r="G31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="28"/>
     </row>
     <row r="32" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="6">
@@ -1284,11 +1290,11 @@
       <c r="D32" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E32" s="25" t="s">
+      <c r="E32" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="F32" s="26"/>
-      <c r="G32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="28"/>
     </row>
     <row r="33" spans="2:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="6">
@@ -1300,14 +1306,14 @@
       <c r="D33" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="25" t="s">
+      <c r="E33" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="F33" s="26"/>
-      <c r="G33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="28"/>
     </row>
     <row r="34" spans="2:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="34">
+      <c r="B34" s="19">
         <v>43164</v>
       </c>
       <c r="C34" s="13" t="s">
@@ -1316,155 +1322,163 @@
       <c r="D34" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E34" s="25" t="s">
+      <c r="E34" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="F34" s="26"/>
-      <c r="G34" s="27"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="8"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="21"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="28"/>
+    </row>
+    <row r="35" spans="2:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B35" s="6">
+        <v>43165</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="F35" s="27"/>
+      <c r="G35" s="28"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="8"/>
       <c r="C36" s="14"/>
       <c r="D36" s="7"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="21"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="22"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="8"/>
       <c r="C37" s="14"/>
       <c r="D37" s="7"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="21"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="22"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" s="8"/>
       <c r="C38" s="14"/>
       <c r="D38" s="7"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="21"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="22"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="8"/>
       <c r="C39" s="14"/>
       <c r="D39" s="7"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="21"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="22"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="8"/>
       <c r="C40" s="14"/>
       <c r="D40" s="7"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="21"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" s="8"/>
       <c r="C41" s="14"/>
       <c r="D41" s="7"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="21"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="22"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" s="8"/>
       <c r="C42" s="14"/>
       <c r="D42" s="7"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="21"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="22"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43" s="8"/>
       <c r="C43" s="14"/>
       <c r="D43" s="7"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="21"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="22"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" s="8"/>
       <c r="C44" s="14"/>
       <c r="D44" s="7"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="21"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="22"/>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" s="8"/>
       <c r="C45" s="14"/>
       <c r="D45" s="7"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="21"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="22"/>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" s="8"/>
       <c r="C46" s="14"/>
       <c r="D46" s="7"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="20"/>
-      <c r="G46" s="21"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="22"/>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B47" s="8"/>
       <c r="C47" s="14"/>
       <c r="D47" s="7"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="20"/>
-      <c r="G47" s="21"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="22"/>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B48" s="8"/>
       <c r="C48" s="14"/>
       <c r="D48" s="7"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="20"/>
-      <c r="G48" s="21"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="22"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="8"/>
       <c r="C49" s="14"/>
       <c r="D49" s="7"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="20"/>
-      <c r="G49" s="21"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="22"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="8"/>
       <c r="C50" s="14"/>
       <c r="D50" s="7"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="20"/>
-      <c r="G50" s="21"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="22"/>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B51" s="8"/>
       <c r="C51" s="14"/>
       <c r="D51" s="7"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="21"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="22"/>
     </row>
     <row r="52" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="9"/>
       <c r="C52" s="15"/>
       <c r="D52" s="10"/>
-      <c r="E52" s="31"/>
-      <c r="F52" s="32"/>
-      <c r="G52" s="33"/>
+      <c r="E52" s="23"/>
+      <c r="F52" s="24"/>
+      <c r="G52" s="25"/>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
@@ -1556,28 +1570,12 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
     <mergeCell ref="B1:G2"/>
     <mergeCell ref="B4:C5"/>
     <mergeCell ref="E30:G30"/>
@@ -1594,12 +1592,28 @@
     <mergeCell ref="E29:G29"/>
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding movement, pawn elimination, victory conditions
</commit_message>
<xml_diff>
--- a/Documentation/MHG_Journal_de_travail_Tablut.xlsx
+++ b/Documentation/MHG_Journal_de_travail_Tablut.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="54">
   <si>
     <t>Date</t>
   </si>
@@ -177,6 +177,15 @@
   </si>
   <si>
     <t>Les type défini si la case est occupée ou non et par qui.</t>
+  </si>
+  <si>
+    <t>5h15</t>
+  </si>
+  <si>
+    <t>Ajout des déplacements et de l'élimination de pièces et des conditions de victoire</t>
+  </si>
+  <si>
+    <t>Les conditions de victoire n'ont pas encore pu être testées.</t>
   </si>
 </sst>
 </file>
@@ -535,6 +544,33 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -543,33 +579,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -853,8 +862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38:G38"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36:G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -938,11 +947,11 @@
       <c r="D8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="33"/>
-      <c r="G8" s="34"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="25"/>
     </row>
     <row r="9" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B9" s="6">
@@ -1344,13 +1353,21 @@
       <c r="F35" s="27"/>
       <c r="G35" s="28"/>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="8"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="22"/>
+    <row r="36" spans="2:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B36" s="6">
+        <v>43167</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E36" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="F36" s="27"/>
+      <c r="G36" s="28"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="8"/>
@@ -1476,9 +1493,9 @@
       <c r="B52" s="9"/>
       <c r="C52" s="15"/>
       <c r="D52" s="10"/>
-      <c r="E52" s="23"/>
-      <c r="F52" s="24"/>
-      <c r="G52" s="25"/>
+      <c r="E52" s="32"/>
+      <c r="F52" s="33"/>
+      <c r="G52" s="34"/>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
@@ -1570,12 +1587,28 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E41:G41"/>
     <mergeCell ref="B1:G2"/>
     <mergeCell ref="B4:C5"/>
     <mergeCell ref="E30:G30"/>
@@ -1592,28 +1625,12 @@
     <mergeCell ref="E29:G29"/>
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Removing game error form, adding game over screen
</commit_message>
<xml_diff>
--- a/Documentation/MHG_Journal_de_travail_Tablut.xlsx
+++ b/Documentation/MHG_Journal_de_travail_Tablut.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="56">
   <si>
     <t>Date</t>
   </si>
@@ -186,6 +186,12 @@
   </si>
   <si>
     <t>Les conditions de victoire n'ont pas encore pu être testées.</t>
+  </si>
+  <si>
+    <t>Ajout de l'écran de fin</t>
+  </si>
+  <si>
+    <t>Le formulaire de "Game_Error" a été retiré, le jeu est désormais fonctionnel, il ne reste qu'a revoir le code et créer un utilisateur spécial pour la base de données.</t>
   </si>
 </sst>
 </file>
@@ -544,6 +550,33 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -552,33 +585,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -862,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36:G36"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -947,11 +953,11 @@
       <c r="D8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="24"/>
-      <c r="G8" s="25"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="34"/>
     </row>
     <row r="9" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B9" s="6">
@@ -1369,13 +1375,21 @@
       <c r="F36" s="27"/>
       <c r="G36" s="28"/>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="8"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="21"/>
-      <c r="G37" s="22"/>
+    <row r="37" spans="2:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="6">
+        <v>43168</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E37" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="F37" s="27"/>
+      <c r="G37" s="28"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" s="8"/>
@@ -1493,9 +1507,9 @@
       <c r="B52" s="9"/>
       <c r="C52" s="15"/>
       <c r="D52" s="10"/>
-      <c r="E52" s="32"/>
-      <c r="F52" s="33"/>
-      <c r="G52" s="34"/>
+      <c r="E52" s="23"/>
+      <c r="F52" s="24"/>
+      <c r="G52" s="25"/>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
@@ -1587,28 +1601,12 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
     <mergeCell ref="B1:G2"/>
     <mergeCell ref="B4:C5"/>
     <mergeCell ref="E30:G30"/>
@@ -1625,12 +1623,28 @@
     <mergeCell ref="E29:G29"/>
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Enbling king to eliminate pawn, adding user to DB, code review.
Code review in DB_Connect.cs and Exception_Invalid_Name.cs
</commit_message>
<xml_diff>
--- a/Documentation/MHG_Journal_de_travail_Tablut.xlsx
+++ b/Documentation/MHG_Journal_de_travail_Tablut.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="58">
   <si>
     <t>Date</t>
   </si>
@@ -192,6 +192,12 @@
   </si>
   <si>
     <t>Le formulaire de "Game_Error" a été retiré, le jeu est désormais fonctionnel, il ne reste qu'a revoir le code et créer un utilisateur spécial pour la base de données.</t>
+  </si>
+  <si>
+    <t>Création d'un utilisateur pour la base de donnée. Correctif du pion roi. Recherche de méthode d'exécution du script sql pour les futurs utilisateurs. Révision du code et des commentaires.</t>
+  </si>
+  <si>
+    <t>Nous n'utilisons plus root pour des questions de 'bonnes pratiques'. Le roi ne permettait pas d'éliminer des attaquants. Les utilisateurs n'utiliseront pas WAMP (comme nous). Il est possible de lancer un script via l'invite de commande Windows. Révision de la classe DB_Connect.cs, Exception_Invalid_Name.cs.</t>
   </si>
 </sst>
 </file>
@@ -869,7 +875,7 @@
   <dimension ref="B1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+      <selection activeCell="E38" sqref="E38:G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1391,13 +1397,21 @@
       <c r="F37" s="27"/>
       <c r="G37" s="28"/>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="8"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="22"/>
+    <row r="38" spans="2:7" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="6">
+        <v>43171</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E38" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="F38" s="27"/>
+      <c r="G38" s="28"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="8"/>

</xml_diff>

<commit_message>
Embedding the files, reviewing the form_Confirmation code.
</commit_message>
<xml_diff>
--- a/Documentation/MHG_Journal_de_travail_Tablut.xlsx
+++ b/Documentation/MHG_Journal_de_travail_Tablut.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="60">
   <si>
     <t>Date</t>
   </si>
@@ -198,6 +198,12 @@
   </si>
   <si>
     <t>Nous n'utilisons plus root pour des questions de 'bonnes pratiques'. Le roi ne permettait pas d'éliminer des attaquants. Les utilisateurs n'utiliseront pas WAMP (comme nous). Il est possible de lancer un script via l'invite de commande Windows. Révision de la classe DB_Connect.cs, Exception_Invalid_Name.cs.</t>
+  </si>
+  <si>
+    <t>Révision du code form_Confirmation.cs. Import des ressources</t>
+  </si>
+  <si>
+    <t>Les ressources sont désormais intégrées au programme et non liées.</t>
   </si>
 </sst>
 </file>
@@ -556,6 +562,33 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -564,33 +597,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -875,7 +881,7 @@
   <dimension ref="B1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38:G38"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -959,11 +965,11 @@
       <c r="D8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="33"/>
-      <c r="G8" s="34"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="25"/>
     </row>
     <row r="9" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B9" s="6">
@@ -1413,13 +1419,21 @@
       <c r="F38" s="27"/>
       <c r="G38" s="28"/>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="8"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="22"/>
+    <row r="39" spans="2:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B39" s="6">
+        <v>43172</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E39" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="F39" s="27"/>
+      <c r="G39" s="28"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="8"/>
@@ -1521,9 +1535,9 @@
       <c r="B52" s="9"/>
       <c r="C52" s="15"/>
       <c r="D52" s="10"/>
-      <c r="E52" s="23"/>
-      <c r="F52" s="24"/>
-      <c r="G52" s="25"/>
+      <c r="E52" s="32"/>
+      <c r="F52" s="33"/>
+      <c r="G52" s="34"/>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
@@ -1615,12 +1629,28 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E41:G41"/>
     <mergeCell ref="B1:G2"/>
     <mergeCell ref="B4:C5"/>
     <mergeCell ref="E30:G30"/>
@@ -1637,28 +1667,12 @@
     <mergeCell ref="E29:G29"/>
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Code review, adding a new Player_Role enum.
</commit_message>
<xml_diff>
--- a/Documentation/MHG_Journal_de_travail_Tablut.xlsx
+++ b/Documentation/MHG_Journal_de_travail_Tablut.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="63">
   <si>
     <t>Date</t>
   </si>
@@ -204,6 +204,15 @@
   </si>
   <si>
     <t>Les ressources sont désormais intégrées au programme et non liées.</t>
+  </si>
+  <si>
+    <t>2h45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Révision du code </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les commentaires on été revus, une énmération a été ajoutée pour simplifier la compréhension. </t>
   </si>
 </sst>
 </file>
@@ -562,6 +571,33 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -570,33 +606,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -880,8 +889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -965,11 +974,11 @@
       <c r="D8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="24"/>
-      <c r="G8" s="25"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="34"/>
     </row>
     <row r="9" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B9" s="6">
@@ -1435,13 +1444,21 @@
       <c r="F39" s="27"/>
       <c r="G39" s="28"/>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="8"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="22"/>
+    <row r="40" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="6">
+        <v>43174</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E40" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="F40" s="27"/>
+      <c r="G40" s="28"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" s="8"/>
@@ -1535,9 +1552,9 @@
       <c r="B52" s="9"/>
       <c r="C52" s="15"/>
       <c r="D52" s="10"/>
-      <c r="E52" s="32"/>
-      <c r="F52" s="33"/>
-      <c r="G52" s="34"/>
+      <c r="E52" s="23"/>
+      <c r="F52" s="24"/>
+      <c r="G52" s="25"/>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
@@ -1629,28 +1646,12 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
     <mergeCell ref="B1:G2"/>
     <mergeCell ref="B4:C5"/>
     <mergeCell ref="E30:G30"/>
@@ -1667,12 +1668,28 @@
     <mergeCell ref="E29:G29"/>
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Addind form before statistics screen
</commit_message>
<xml_diff>
--- a/Documentation/MHG_Journal_de_travail_Tablut.xlsx
+++ b/Documentation/MHG_Journal_de_travail_Tablut.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="66">
   <si>
     <t>Date</t>
   </si>
@@ -213,6 +213,15 @@
   </si>
   <si>
     <t xml:space="preserve">Les commentaires on été revus, une énmération a été ajoutée pour simplifier la compréhension. </t>
+  </si>
+  <si>
+    <t>2h30</t>
+  </si>
+  <si>
+    <t>Renommage des contrôles, ajout d'un formulaire avant les statistiques en fin de partie. Essais de musique d'ambiance.</t>
+  </si>
+  <si>
+    <t>Ce formulaire permet de pouvoir observer l'état final du plateau. Les musiques d'ambiance n'ont pas encore pu être implémentée.</t>
   </si>
 </sst>
 </file>
@@ -571,6 +580,33 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -579,33 +615,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -890,7 +899,7 @@
   <dimension ref="B1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+      <selection activeCell="E41" sqref="E41:G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -974,11 +983,11 @@
       <c r="D8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="33"/>
-      <c r="G8" s="34"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="25"/>
     </row>
     <row r="9" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B9" s="6">
@@ -1460,17 +1469,25 @@
       <c r="F40" s="27"/>
       <c r="G40" s="28"/>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="8"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="22"/>
+    <row r="41" spans="2:7" ht="63" x14ac:dyDescent="0.25">
+      <c r="B41" s="6">
+        <v>43174</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E41" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="F41" s="27"/>
+      <c r="G41" s="28"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" s="8"/>
-      <c r="C42" s="14"/>
+      <c r="C42" s="13"/>
       <c r="D42" s="7"/>
       <c r="E42" s="20"/>
       <c r="F42" s="21"/>
@@ -1552,9 +1569,9 @@
       <c r="B52" s="9"/>
       <c r="C52" s="15"/>
       <c r="D52" s="10"/>
-      <c r="E52" s="23"/>
-      <c r="F52" s="24"/>
-      <c r="G52" s="25"/>
+      <c r="E52" s="32"/>
+      <c r="F52" s="33"/>
+      <c r="G52" s="34"/>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
@@ -1646,12 +1663,28 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E41:G41"/>
     <mergeCell ref="B1:G2"/>
     <mergeCell ref="B4:C5"/>
     <mergeCell ref="E30:G30"/>
@@ -1668,28 +1701,12 @@
     <mergeCell ref="E29:G29"/>
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Making tests and correcting some small errors
</commit_message>
<xml_diff>
--- a/Documentation/MHG_Journal_de_travail_Tablut.xlsx
+++ b/Documentation/MHG_Journal_de_travail_Tablut.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="71">
   <si>
     <t>Date</t>
   </si>
@@ -595,6 +595,33 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -603,33 +630,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -914,7 +914,7 @@
   <dimension ref="B1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44:G44"/>
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -998,11 +998,11 @@
       <c r="D8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="33"/>
-      <c r="G8" s="34"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="25"/>
     </row>
     <row r="9" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B9" s="6">
@@ -1547,9 +1547,15 @@
       <c r="G44" s="22"/>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="8"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="7"/>
+      <c r="B45" s="6">
+        <v>43181</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>51</v>
+      </c>
       <c r="E45" s="20"/>
       <c r="F45" s="21"/>
       <c r="G45" s="22"/>
@@ -1606,9 +1612,9 @@
       <c r="B52" s="9"/>
       <c r="C52" s="15"/>
       <c r="D52" s="10"/>
-      <c r="E52" s="23"/>
-      <c r="F52" s="24"/>
-      <c r="G52" s="25"/>
+      <c r="E52" s="32"/>
+      <c r="F52" s="33"/>
+      <c r="G52" s="34"/>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
@@ -1700,12 +1706,28 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E41:G41"/>
     <mergeCell ref="B1:G2"/>
     <mergeCell ref="B4:C5"/>
     <mergeCell ref="E30:G30"/>
@@ -1722,28 +1744,12 @@
     <mergeCell ref="E29:G29"/>
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Generating code doc, beginning class diagram
</commit_message>
<xml_diff>
--- a/Documentation/MHG_Journal_de_travail_Tablut.xlsx
+++ b/Documentation/MHG_Journal_de_travail_Tablut.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="75">
   <si>
     <t>Date</t>
   </si>
@@ -240,6 +240,15 @@
   </si>
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>Les test sont terminés.</t>
+  </si>
+  <si>
+    <t>Documentation du code. Diagramme de classes.</t>
+  </si>
+  <si>
+    <t>Génération de la documentation du code. Début de réalisation du diagramme de classe.</t>
   </si>
 </sst>
 </file>
@@ -598,6 +607,33 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -606,33 +642,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -917,7 +926,7 @@
   <dimension ref="B1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1001,11 +1010,11 @@
       <c r="D8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="33"/>
-      <c r="G8" s="34"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="25"/>
     </row>
     <row r="9" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B9" s="6">
@@ -1573,17 +1582,27 @@
       <c r="D46" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E46" s="20"/>
+      <c r="E46" s="20" t="s">
+        <v>72</v>
+      </c>
       <c r="F46" s="21"/>
       <c r="G46" s="22"/>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B47" s="8"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="7"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="21"/>
-      <c r="G47" s="22"/>
+    <row r="47" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B47" s="6">
+        <v>43185</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E47" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="F47" s="27"/>
+      <c r="G47" s="28"/>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B48" s="8"/>
@@ -1621,9 +1640,9 @@
       <c r="B52" s="9"/>
       <c r="C52" s="15"/>
       <c r="D52" s="10"/>
-      <c r="E52" s="23"/>
-      <c r="F52" s="24"/>
-      <c r="G52" s="25"/>
+      <c r="E52" s="32"/>
+      <c r="F52" s="33"/>
+      <c r="G52" s="34"/>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
@@ -1715,12 +1734,28 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E41:G41"/>
     <mergeCell ref="B1:G2"/>
     <mergeCell ref="B4:C5"/>
     <mergeCell ref="E30:G30"/>
@@ -1737,28 +1772,12 @@
     <mergeCell ref="E29:G29"/>
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Making class diagram picture, adding flux diagram and updating doc
</commit_message>
<xml_diff>
--- a/Documentation/MHG_Journal_de_travail_Tablut.xlsx
+++ b/Documentation/MHG_Journal_de_travail_Tablut.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="85">
   <si>
     <t>Date</t>
   </si>
@@ -255,6 +255,30 @@
   </si>
   <si>
     <t>Il y aura deux diagrammes de classes pour des raisons de mise en page sur la documentation finale.</t>
+  </si>
+  <si>
+    <t>Creation d'image pour la documentation.</t>
+  </si>
+  <si>
+    <t>Image du diagramme de classe et des maquettes.</t>
+  </si>
+  <si>
+    <t>Ajustelement d'une règle d'élimination.</t>
+  </si>
+  <si>
+    <t>10 minutes</t>
+  </si>
+  <si>
+    <t>Le rois ne pouvait pas être éliminé si adjacent au trone. Pourtant il est expliqué explicitement qu'il est possible. Cependant les règles sont approximatives, il y a donc des moyens pour ne pas être éliminé (laisser un pion dans un coin p.ex.).</t>
+  </si>
+  <si>
+    <t>Diagramme de flux</t>
+  </si>
+  <si>
+    <t>Réalisation de diagrame de flux pour le cœur du projet: Sélection des pions, élimination, détection de fin de partie…</t>
+  </si>
+  <si>
+    <t>Rédaction documentation</t>
   </si>
 </sst>
 </file>
@@ -549,7 +573,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -568,12 +592,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -613,6 +631,33 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -622,32 +667,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -931,8 +952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -946,22 +967,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="2" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
     </row>
     <row r="3" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
@@ -972,18 +993,18 @@
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="30"/>
+      <c r="C4" s="28"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -991,672 +1012,702 @@
     </row>
     <row r="6" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
     </row>
     <row r="8" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
         <v>43129</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="33"/>
-      <c r="G8" s="34"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="23"/>
     </row>
     <row r="9" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B9" s="6">
         <v>43130</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="11" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="22"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="20"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="6">
         <v>43130</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="11" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="18"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="16"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>43132</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="12" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="22"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="20"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
         <v>43132</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="12" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="18"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="16"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="6">
         <v>43133</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="12" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="18"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="16"/>
     </row>
     <row r="14" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="6">
         <v>43133</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="26"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="28"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="26"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="6">
         <v>43136</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="20"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="22"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="20"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="6">
         <v>43137</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="20"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="22"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="20"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="6">
         <v>43139</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="16"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="18"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="16"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="6">
         <v>43139</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="20"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="22"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="20"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="6">
         <v>43139</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="12" t="s">
         <v>26</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="20"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="22"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="20"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="6">
         <v>43140</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="12" t="s">
         <v>25</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="E20" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="F20" s="21"/>
-      <c r="G20" s="22"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="20"/>
     </row>
     <row r="21" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B21" s="6">
         <v>43143</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="11" t="s">
         <v>24</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="20"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="22"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="20"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="6">
         <v>43143</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="20"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="22"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="20"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="6">
         <v>43144</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="20"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="22"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="20"/>
     </row>
     <row r="24" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B24" s="6">
         <v>43146</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="11" t="s">
         <v>39</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="26" t="s">
+      <c r="E24" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="F24" s="27"/>
-      <c r="G24" s="28"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="26"/>
     </row>
     <row r="25" spans="2:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="6">
         <v>43147</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="12" t="s">
         <v>33</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E25" s="26" t="s">
+      <c r="E25" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="F25" s="27"/>
-      <c r="G25" s="28"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="26"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="6">
         <v>43147</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="12" t="s">
         <v>34</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="20"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="22"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="20"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="6">
         <v>43157</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="20" t="s">
+      <c r="E27" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="21"/>
-      <c r="G27" s="22"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="20"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="6">
         <v>43158</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="E28" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="F28" s="21"/>
-      <c r="G28" s="22"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="20"/>
     </row>
     <row r="29" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="6">
         <v>43160</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="26" t="s">
+      <c r="E29" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="27"/>
-      <c r="G29" s="28"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="26"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="6">
         <v>43160</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="12" t="s">
         <v>40</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E30" s="20"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="22"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="20"/>
     </row>
     <row r="31" spans="2:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="6">
         <v>43160</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="12" t="s">
         <v>41</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="26" t="s">
+      <c r="E31" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="F31" s="27"/>
-      <c r="G31" s="28"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="26"/>
     </row>
     <row r="32" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="6">
         <v>43161</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="12" t="s">
         <v>43</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E32" s="26" t="s">
+      <c r="E32" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="F32" s="27"/>
-      <c r="G32" s="28"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="26"/>
     </row>
     <row r="33" spans="2:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="6">
         <v>43161</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="12" t="s">
         <v>45</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="26" t="s">
+      <c r="E33" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="F33" s="27"/>
-      <c r="G33" s="28"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="26"/>
     </row>
     <row r="34" spans="2:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="19">
+      <c r="B34" s="17">
         <v>43164</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="11" t="s">
         <v>47</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E34" s="26" t="s">
+      <c r="E34" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="F34" s="27"/>
-      <c r="G34" s="28"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="26"/>
     </row>
     <row r="35" spans="2:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B35" s="6">
         <v>43165</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="11" t="s">
         <v>49</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E35" s="26" t="s">
+      <c r="E35" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="F35" s="27"/>
-      <c r="G35" s="28"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="26"/>
     </row>
     <row r="36" spans="2:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B36" s="6">
         <v>43167</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C36" s="11" t="s">
         <v>52</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E36" s="26" t="s">
+      <c r="E36" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F36" s="27"/>
-      <c r="G36" s="28"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="26"/>
     </row>
     <row r="37" spans="2:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="6">
         <v>43168</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C37" s="12" t="s">
         <v>54</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E37" s="26" t="s">
+      <c r="E37" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="F37" s="27"/>
-      <c r="G37" s="28"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="26"/>
     </row>
     <row r="38" spans="2:7" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="6">
         <v>43171</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C38" s="11" t="s">
         <v>56</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E38" s="26" t="s">
+      <c r="E38" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="F38" s="27"/>
-      <c r="G38" s="28"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="26"/>
     </row>
     <row r="39" spans="2:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B39" s="6">
         <v>43172</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="11" t="s">
         <v>58</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E39" s="26" t="s">
+      <c r="E39" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="F39" s="27"/>
-      <c r="G39" s="28"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="26"/>
     </row>
     <row r="40" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="6">
         <v>43174</v>
       </c>
-      <c r="C40" s="14" t="s">
+      <c r="C40" s="12" t="s">
         <v>61</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E40" s="26" t="s">
+      <c r="E40" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="F40" s="27"/>
-      <c r="G40" s="28"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="26"/>
     </row>
     <row r="41" spans="2:7" ht="63" x14ac:dyDescent="0.25">
       <c r="B41" s="6">
         <v>43174</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="C41" s="11" t="s">
         <v>64</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E41" s="26" t="s">
+      <c r="E41" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="F41" s="27"/>
-      <c r="G41" s="28"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="26"/>
     </row>
     <row r="42" spans="2:7" ht="63" x14ac:dyDescent="0.25">
       <c r="B42" s="6">
         <v>43175</v>
       </c>
-      <c r="C42" s="13" t="s">
+      <c r="C42" s="11" t="s">
         <v>66</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E42" s="26" t="s">
+      <c r="E42" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="F42" s="27"/>
-      <c r="G42" s="28"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="26"/>
     </row>
     <row r="43" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B43" s="6">
         <v>43178</v>
       </c>
-      <c r="C43" s="13" t="s">
+      <c r="C43" s="11" t="s">
         <v>68</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E43" s="26" t="s">
+      <c r="E43" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="F43" s="27"/>
-      <c r="G43" s="28"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="26"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" s="6">
         <v>43179</v>
       </c>
-      <c r="C44" s="14" t="s">
+      <c r="C44" s="12" t="s">
         <v>70</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E44" s="20"/>
-      <c r="F44" s="21"/>
-      <c r="G44" s="22"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="20"/>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" s="6">
         <v>43181</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="C45" s="12" t="s">
         <v>70</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="E45" s="20"/>
-      <c r="F45" s="21"/>
-      <c r="G45" s="22"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="20"/>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" s="6">
         <v>43182</v>
       </c>
-      <c r="C46" s="14" t="s">
+      <c r="C46" s="12" t="s">
         <v>71</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E46" s="20" t="s">
+      <c r="E46" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="F46" s="21"/>
-      <c r="G46" s="22"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="20"/>
     </row>
     <row r="47" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B47" s="6">
         <v>43185</v>
       </c>
-      <c r="C47" s="13" t="s">
+      <c r="C47" s="11" t="s">
         <v>73</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E47" s="26" t="s">
+      <c r="E47" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="F47" s="27"/>
-      <c r="G47" s="28"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="26"/>
     </row>
     <row r="48" spans="2:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="6">
         <v>43186</v>
       </c>
-      <c r="C48" s="14" t="s">
+      <c r="C48" s="12" t="s">
         <v>75</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E48" s="26" t="s">
+      <c r="E48" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="F48" s="27"/>
-      <c r="G48" s="28"/>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B49" s="8"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="7"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="21"/>
-      <c r="G49" s="22"/>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B50" s="8"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="22"/>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B51" s="8"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="7"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="21"/>
-      <c r="G51" s="22"/>
+      <c r="F48" s="25"/>
+      <c r="G48" s="26"/>
+    </row>
+    <row r="49" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B49" s="6">
+        <v>43188</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E49" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="F49" s="19"/>
+      <c r="G49" s="20"/>
+    </row>
+    <row r="50" spans="2:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="6">
+        <v>43188</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E50" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="F50" s="25"/>
+      <c r="G50" s="26"/>
+    </row>
+    <row r="51" spans="2:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="6">
+        <v>43188</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E51" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="F51" s="25"/>
+      <c r="G51" s="26"/>
     </row>
     <row r="52" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="9"/>
-      <c r="C52" s="15"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="23"/>
-      <c r="F52" s="24"/>
-      <c r="G52" s="25"/>
+      <c r="B52" s="33">
+        <v>43188</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52" s="30"/>
+      <c r="F52" s="31"/>
+      <c r="G52" s="32"/>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
@@ -1748,12 +1799,28 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E41:G41"/>
     <mergeCell ref="B1:G2"/>
     <mergeCell ref="B4:C5"/>
     <mergeCell ref="E30:G30"/>
@@ -1770,28 +1837,12 @@
     <mergeCell ref="E29:G29"/>
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Documentation update and adjustments
</commit_message>
<xml_diff>
--- a/Documentation/MHG_Journal_de_travail_Tablut.xlsx
+++ b/Documentation/MHG_Journal_de_travail_Tablut.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="88">
   <si>
     <t>Date</t>
   </si>
@@ -278,7 +278,16 @@
     <t>Réalisation de diagrame de flux pour le cœur du projet: Sélection des pions, élimination, détection de fin de partie…</t>
   </si>
   <si>
-    <t>Rédaction documentation</t>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>Rédaction documentation.</t>
+  </si>
+  <si>
+    <t>Ajustements.</t>
+  </si>
+  <si>
+    <t>Certaines fenêtres pouvaient être agrandies alors que non. Ajout d'un try catch sur une zone de mise à jour de la base de données. Ajout des sons sur le bouton du volume. Création d'un dossier rendu. Correctif, lorsque le roi peut s'auto-éliminer. Relecture de la documentation.</t>
   </si>
 </sst>
 </file>
@@ -573,10 +582,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -622,6 +629,9 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -631,6 +641,33 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -640,35 +677,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -950,10 +966,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G63"/>
+  <dimension ref="B1:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56:G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -967,860 +983,962 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
     </row>
     <row r="2" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
     </row>
     <row r="3" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
     </row>
     <row r="5" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
     </row>
     <row r="6" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
     </row>
     <row r="8" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B8" s="4">
+      <c r="B8" s="2">
         <v>43129</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="22"/>
-      <c r="G8" s="23"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="31"/>
     </row>
     <row r="9" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B9" s="6">
+      <c r="B9" s="4">
         <v>43130</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="20"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="6">
+      <c r="B10" s="4">
         <v>43130</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="16"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="14"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="6">
+      <c r="B11" s="4">
         <v>43132</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="18"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="20"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="19"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="6">
+      <c r="B12" s="4">
         <v>43132</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="16"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="14"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="6">
+      <c r="B13" s="4">
         <v>43133</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="16"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="14"/>
     </row>
     <row r="14" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="6">
+      <c r="B14" s="4">
         <v>43133</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="24"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="26"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="22"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="6">
+      <c r="B15" s="4">
         <v>43136</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="18"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="20"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="19"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="6">
+      <c r="B16" s="4">
         <v>43137</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="18"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="20"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="19"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="6">
+      <c r="B17" s="4">
         <v>43139</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="14"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="16"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="14"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="6">
+      <c r="B18" s="4">
         <v>43139</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="18"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="20"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="19"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="6">
+      <c r="B19" s="4">
         <v>43139</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="18"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="20"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="19"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="6">
+      <c r="B20" s="4">
         <v>43140</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="F20" s="19"/>
-      <c r="G20" s="20"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="19"/>
     </row>
     <row r="21" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B21" s="6">
+      <c r="B21" s="4">
         <v>43143</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="18"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="20"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="19"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="6">
+      <c r="B22" s="4">
         <v>43143</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="18"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="20"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="19"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="6">
+      <c r="B23" s="4">
         <v>43144</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="18"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="20"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="19"/>
     </row>
     <row r="24" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B24" s="6">
+      <c r="B24" s="4">
         <v>43146</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="24" t="s">
+      <c r="E24" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="F24" s="25"/>
-      <c r="G24" s="26"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="22"/>
     </row>
     <row r="25" spans="2:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="6">
+      <c r="B25" s="4">
         <v>43147</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E25" s="24" t="s">
+      <c r="E25" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="F25" s="25"/>
-      <c r="G25" s="26"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="22"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="6">
+      <c r="B26" s="4">
         <v>43147</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="18"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="20"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="19"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="6">
+      <c r="B27" s="4">
         <v>43157</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="18" t="s">
+      <c r="E27" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="19"/>
-      <c r="G27" s="20"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="19"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="6">
+      <c r="B28" s="4">
         <v>43158</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E28" s="18" t="s">
+      <c r="E28" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="F28" s="19"/>
-      <c r="G28" s="20"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="19"/>
     </row>
     <row r="29" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="6">
+      <c r="B29" s="4">
         <v>43160</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="24" t="s">
+      <c r="E29" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="25"/>
-      <c r="G29" s="26"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="22"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="6">
+      <c r="B30" s="4">
         <v>43160</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E30" s="18"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="20"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="19"/>
     </row>
     <row r="31" spans="2:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="6">
+      <c r="B31" s="4">
         <v>43160</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="24" t="s">
+      <c r="E31" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="F31" s="25"/>
-      <c r="G31" s="26"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="22"/>
     </row>
     <row r="32" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="6">
+      <c r="B32" s="4">
         <v>43161</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E32" s="24" t="s">
+      <c r="E32" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="F32" s="25"/>
-      <c r="G32" s="26"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="22"/>
     </row>
     <row r="33" spans="2:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="6">
+      <c r="B33" s="4">
         <v>43161</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="24" t="s">
+      <c r="E33" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="F33" s="25"/>
-      <c r="G33" s="26"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="22"/>
     </row>
     <row r="34" spans="2:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="17">
+      <c r="B34" s="15">
         <v>43164</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E34" s="24" t="s">
+      <c r="E34" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="F34" s="25"/>
-      <c r="G34" s="26"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="22"/>
     </row>
     <row r="35" spans="2:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B35" s="6">
+      <c r="B35" s="4">
         <v>43165</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E35" s="24" t="s">
+      <c r="E35" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="F35" s="25"/>
-      <c r="G35" s="26"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="22"/>
     </row>
     <row r="36" spans="2:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B36" s="6">
+      <c r="B36" s="4">
         <v>43167</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E36" s="24" t="s">
+      <c r="E36" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F36" s="25"/>
-      <c r="G36" s="26"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="22"/>
     </row>
     <row r="37" spans="2:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="6">
+      <c r="B37" s="4">
         <v>43168</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C37" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E37" s="24" t="s">
+      <c r="E37" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="F37" s="25"/>
-      <c r="G37" s="26"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="22"/>
     </row>
     <row r="38" spans="2:7" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="6">
+      <c r="B38" s="4">
         <v>43171</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E38" s="24" t="s">
+      <c r="E38" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="F38" s="25"/>
-      <c r="G38" s="26"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="22"/>
     </row>
     <row r="39" spans="2:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B39" s="6">
+      <c r="B39" s="4">
         <v>43172</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E39" s="24" t="s">
+      <c r="E39" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="F39" s="25"/>
-      <c r="G39" s="26"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="22"/>
     </row>
     <row r="40" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="6">
+      <c r="B40" s="4">
         <v>43174</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C40" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E40" s="24" t="s">
+      <c r="E40" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="F40" s="25"/>
-      <c r="G40" s="26"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="22"/>
     </row>
     <row r="41" spans="2:7" ht="63" x14ac:dyDescent="0.25">
-      <c r="B41" s="6">
+      <c r="B41" s="4">
         <v>43174</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E41" s="24" t="s">
+      <c r="E41" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="F41" s="25"/>
-      <c r="G41" s="26"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="22"/>
     </row>
     <row r="42" spans="2:7" ht="63" x14ac:dyDescent="0.25">
-      <c r="B42" s="6">
+      <c r="B42" s="4">
         <v>43175</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D42" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E42" s="24" t="s">
+      <c r="E42" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="F42" s="25"/>
-      <c r="G42" s="26"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="22"/>
     </row>
     <row r="43" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B43" s="6">
+      <c r="B43" s="4">
         <v>43178</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C43" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E43" s="24" t="s">
+      <c r="E43" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="F43" s="25"/>
-      <c r="G43" s="26"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="22"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="6">
+      <c r="B44" s="4">
         <v>43179</v>
       </c>
-      <c r="C44" s="12" t="s">
+      <c r="C44" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E44" s="18"/>
-      <c r="F44" s="19"/>
-      <c r="G44" s="20"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="19"/>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="6">
+      <c r="B45" s="4">
         <v>43181</v>
       </c>
-      <c r="C45" s="12" t="s">
+      <c r="C45" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D45" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E45" s="18"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="20"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="19"/>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="6">
+      <c r="B46" s="4">
         <v>43182</v>
       </c>
-      <c r="C46" s="12" t="s">
+      <c r="C46" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="D46" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E46" s="18" t="s">
+      <c r="E46" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="F46" s="19"/>
-      <c r="G46" s="20"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="19"/>
     </row>
     <row r="47" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B47" s="6">
+      <c r="B47" s="4">
         <v>43185</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C47" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="D47" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E47" s="24" t="s">
+      <c r="E47" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="F47" s="25"/>
-      <c r="G47" s="26"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="22"/>
     </row>
     <row r="48" spans="2:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="6">
+      <c r="B48" s="4">
         <v>43186</v>
       </c>
-      <c r="C48" s="12" t="s">
+      <c r="C48" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D48" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E48" s="24" t="s">
+      <c r="E48" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="F48" s="25"/>
-      <c r="G48" s="26"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="22"/>
     </row>
     <row r="49" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B49" s="6">
+      <c r="B49" s="4">
         <v>43188</v>
       </c>
-      <c r="C49" s="11" t="s">
+      <c r="C49" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D49" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E49" s="18" t="s">
+      <c r="E49" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="F49" s="19"/>
-      <c r="G49" s="20"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="19"/>
     </row>
     <row r="50" spans="2:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="6">
+      <c r="B50" s="4">
         <v>43188</v>
       </c>
-      <c r="C50" s="11" t="s">
+      <c r="C50" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D50" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E50" s="24" t="s">
+      <c r="E50" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="F50" s="25"/>
-      <c r="G50" s="26"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="22"/>
     </row>
     <row r="51" spans="2:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="6">
+      <c r="B51" s="4">
         <v>43188</v>
       </c>
-      <c r="C51" s="12" t="s">
+      <c r="C51" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D51" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E51" s="24" t="s">
+      <c r="E51" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="F51" s="25"/>
-      <c r="G51" s="26"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="22"/>
     </row>
     <row r="52" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="33">
+      <c r="B52" s="16">
         <v>43188</v>
       </c>
-      <c r="C52" s="13" t="s">
+      <c r="C52" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52" s="23"/>
+      <c r="F52" s="24"/>
+      <c r="G52" s="25"/>
+    </row>
+    <row r="53" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="16">
+        <v>43201</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D53" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="D52" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E52" s="30"/>
-      <c r="F52" s="31"/>
-      <c r="G52" s="32"/>
-    </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
-    </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
-    </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="2"/>
-    </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
-    </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-      <c r="G57" s="2"/>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
-      <c r="G58" s="2"/>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
-      <c r="G59" s="2"/>
-    </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
-      <c r="G60" s="2"/>
-    </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
-      <c r="G61" s="2"/>
-    </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="2"/>
-      <c r="F62" s="2"/>
-      <c r="G62" s="2"/>
-    </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
-      <c r="G63" s="2"/>
+      <c r="E53" s="23"/>
+      <c r="F53" s="24"/>
+      <c r="G53" s="25"/>
+    </row>
+    <row r="54" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="16">
+        <v>43202</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E54" s="23"/>
+      <c r="F54" s="24"/>
+      <c r="G54" s="25"/>
+    </row>
+    <row r="55" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="16">
+        <v>43203</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E55" s="23"/>
+      <c r="F55" s="24"/>
+      <c r="G55" s="25"/>
+    </row>
+    <row r="56" spans="2:7" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="16">
+        <v>43206</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E56" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="F56" s="33"/>
+      <c r="G56" s="34"/>
+    </row>
+    <row r="57" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="16"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="23"/>
+      <c r="F57" s="24"/>
+      <c r="G57" s="25"/>
+    </row>
+    <row r="58" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="16"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="23"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="25"/>
+    </row>
+    <row r="59" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="16"/>
+      <c r="C59" s="11"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="23"/>
+      <c r="F59" s="24"/>
+      <c r="G59" s="25"/>
+    </row>
+    <row r="60" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="16"/>
+      <c r="C60" s="11"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="23"/>
+      <c r="F60" s="24"/>
+      <c r="G60" s="25"/>
+    </row>
+    <row r="61" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="16"/>
+      <c r="C61" s="11"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="23"/>
+      <c r="F61" s="24"/>
+      <c r="G61" s="25"/>
+    </row>
+    <row r="62" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="16"/>
+      <c r="C62" s="11"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="23"/>
+      <c r="F62" s="24"/>
+      <c r="G62" s="25"/>
+    </row>
+    <row r="63" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="16"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="23"/>
+      <c r="F63" s="24"/>
+      <c r="G63" s="25"/>
+    </row>
+    <row r="64" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="16"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="23"/>
+      <c r="F64" s="24"/>
+      <c r="G64" s="25"/>
+    </row>
+    <row r="65" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="16"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="23"/>
+      <c r="F65" s="24"/>
+      <c r="G65" s="25"/>
+    </row>
+    <row r="66" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="16"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="23"/>
+      <c r="F66" s="24"/>
+      <c r="G66" s="25"/>
+    </row>
+    <row r="67" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="16"/>
+      <c r="C67" s="11"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="23"/>
+      <c r="F67" s="24"/>
+      <c r="G67" s="25"/>
+    </row>
+    <row r="68" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="16"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="23"/>
+      <c r="F68" s="24"/>
+      <c r="G68" s="25"/>
+    </row>
+    <row r="69" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="16"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="23"/>
+      <c r="F69" s="24"/>
+      <c r="G69" s="25"/>
+    </row>
+    <row r="70" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="16"/>
+      <c r="C70" s="11"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="23"/>
+      <c r="F70" s="24"/>
+      <c r="G70" s="25"/>
+    </row>
+    <row r="71" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="16"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="23"/>
+      <c r="F71" s="24"/>
+      <c r="G71" s="25"/>
+    </row>
+    <row r="72" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="16"/>
+      <c r="C72" s="11"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="23"/>
+      <c r="F72" s="24"/>
+      <c r="G72" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="44">
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="E41:G41"/>
+  <mergeCells count="64">
+    <mergeCell ref="E68:G68"/>
+    <mergeCell ref="E69:G69"/>
+    <mergeCell ref="E70:G70"/>
+    <mergeCell ref="E71:G71"/>
+    <mergeCell ref="E72:G72"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="E64:G64"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="E66:G66"/>
+    <mergeCell ref="E67:G67"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="E59:G59"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="E61:G61"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
     <mergeCell ref="B1:G2"/>
     <mergeCell ref="B4:C5"/>
     <mergeCell ref="E30:G30"/>
@@ -1837,12 +1955,28 @@
     <mergeCell ref="E29:G29"/>
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="E7:G7"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="E52:G52"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="E48:G48"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ending documentation, updating comments.
</commit_message>
<xml_diff>
--- a/Documentation/MHG_Journal_de_travail_Tablut.xlsx
+++ b/Documentation/MHG_Journal_de_travail_Tablut.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$G$59</definedName>
+  </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="93">
   <si>
     <t>Date</t>
   </si>
@@ -125,159 +128,45 @@
     <t>30 min</t>
   </si>
   <si>
-    <t>Création de profil.</t>
-  </si>
-  <si>
-    <t>Création UI gestion de profil.</t>
-  </si>
-  <si>
     <t>Permet de savoir si un profil existe déjà, si la syntaxe du nom est correct ou si le serveur de base de données est allumé.</t>
   </si>
   <si>
-    <t>Gestion de profils fonctionnelle avec messages d'erreurs en cas de mauvaise manipulation.</t>
-  </si>
-  <si>
     <t>En cours.</t>
   </si>
   <si>
-    <t>Logique gestion de profil.</t>
-  </si>
-  <si>
-    <t>Création UI de création de profil, création de profil</t>
-  </si>
-  <si>
-    <t>Création UI Sélection des joueurs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Logique sélection des joueurs </t>
-  </si>
-  <si>
-    <t>En cours, les drop down list se remplissent. Il faut encore ajouter une erreur si deux même profils sont choisis</t>
-  </si>
-  <si>
-    <t>Fin logique sélection des joueurs</t>
-  </si>
-  <si>
-    <t>Les jouers doivent être sélectionnés pour lancer une partie. Doublon impossible</t>
-  </si>
-  <si>
-    <t>Prototype de remplissage de grille</t>
-  </si>
-  <si>
-    <t>Un table layout panel a été placé au dessous du dessin du plateau, de ce fait il sera possible de placer les pions en fonctions d'une ligne et d'une colonne.</t>
-  </si>
-  <si>
-    <t>Ajout des pièces sur le plateau, considération des futures classes à ajouter.</t>
-  </si>
-  <si>
-    <t>Une classe Square, héritée de picture box a été créée, elle inclut une énumération personnalisée.</t>
-  </si>
-  <si>
-    <t>Ajout des classes "Game" et "Joueur". De plus les cases ont désormais un type.</t>
-  </si>
-  <si>
     <t>Les type défini si la case est occupée ou non et par qui.</t>
   </si>
   <si>
     <t>5h15</t>
   </si>
   <si>
-    <t>Ajout des déplacements et de l'élimination de pièces et des conditions de victoire</t>
-  </si>
-  <si>
     <t>Les conditions de victoire n'ont pas encore pu être testées.</t>
   </si>
   <si>
-    <t>Ajout de l'écran de fin</t>
-  </si>
-  <si>
-    <t>Le formulaire de "Game_Error" a été retiré, le jeu est désormais fonctionnel, il ne reste qu'a revoir le code et créer un utilisateur spécial pour la base de données.</t>
-  </si>
-  <si>
-    <t>Création d'un utilisateur pour la base de donnée. Correctif du pion roi. Recherche de méthode d'exécution du script sql pour les futurs utilisateurs. Révision du code et des commentaires.</t>
-  </si>
-  <si>
     <t>Nous n'utilisons plus root pour des questions de 'bonnes pratiques'. Le roi ne permettait pas d'éliminer des attaquants. Les utilisateurs n'utiliseront pas WAMP (comme nous). Il est possible de lancer un script via l'invite de commande Windows. Révision de la classe DB_Connect.cs, Exception_Invalid_Name.cs.</t>
   </si>
   <si>
-    <t>Révision du code form_Confirmation.cs. Import des ressources</t>
-  </si>
-  <si>
     <t>Les ressources sont désormais intégrées au programme et non liées.</t>
   </si>
   <si>
     <t>2h45</t>
   </si>
   <si>
-    <t xml:space="preserve">Révision du code </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Les commentaires on été revus, une énmération a été ajoutée pour simplifier la compréhension. </t>
-  </si>
-  <si>
     <t>2h30</t>
   </si>
   <si>
     <t>Renommage des contrôles, ajout d'un formulaire avant les statistiques en fin de partie. Essais de musique d'ambiance.</t>
   </si>
   <si>
-    <t>Ce formulaire permet de pouvoir observer l'état final du plateau. Les musiques d'ambiance n'ont pas encore pu être implémentée.</t>
-  </si>
-  <si>
-    <t>Tests de création d'un installer dans un programme parrallèle de test et test d'ajout de music d'arrière plan</t>
-  </si>
-  <si>
-    <t>L'installeur installe toutes les dépendances. Reste à ajouter les modification sur le projet de base.</t>
-  </si>
-  <si>
-    <t>Ajout musique d'ambiance et ajout du "Setup project"</t>
-  </si>
-  <si>
     <t>Le setup project permet la création d'un installeur.</t>
   </si>
   <si>
-    <t>Tests</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>Les test sont terminés.</t>
-  </si>
-  <si>
     <t>Documentation du code. Diagramme de classes.</t>
   </si>
   <si>
     <t>Génération de la documentation du code. Début de réalisation du diagramme de classe.</t>
   </si>
   <si>
-    <t>Diagramme de classes.</t>
-  </si>
-  <si>
-    <t>Il y aura deux diagrammes de classes pour des raisons de mise en page sur la documentation finale.</t>
-  </si>
-  <si>
-    <t>Creation d'image pour la documentation.</t>
-  </si>
-  <si>
-    <t>Image du diagramme de classe et des maquettes.</t>
-  </si>
-  <si>
-    <t>Ajustelement d'une règle d'élimination.</t>
-  </si>
-  <si>
-    <t>10 minutes</t>
-  </si>
-  <si>
-    <t>Le rois ne pouvait pas être éliminé si adjacent au trone. Pourtant il est expliqué explicitement qu'il est possible. Cependant les règles sont approximatives, il y a donc des moyens pour ne pas être éliminé (laisser un pion dans un coin p.ex.).</t>
-  </si>
-  <si>
-    <t>Diagramme de flux</t>
-  </si>
-  <si>
-    <t>Réalisation de diagrame de flux pour le cœur du projet: Sélection des pions, élimination, détection de fin de partie…</t>
-  </si>
-  <si>
     <t>2h</t>
   </si>
   <si>
@@ -287,13 +176,136 @@
     <t>Ajustements.</t>
   </si>
   <si>
-    <t>Certaines fenêtres pouvaient être agrandies alors que non. Ajout d'un try catch sur une zone de mise à jour de la base de données. Ajout des sons sur le bouton du volume. Création d'un dossier rendu. Correctif, lorsque le roi peut s'auto-éliminer. Relecture de la documentation.</t>
-  </si>
-  <si>
     <t>Relecture de la documentation.</t>
   </si>
   <si>
     <t>23/115 pages ont été relues.</t>
+  </si>
+  <si>
+    <t>Création UI de création de profils. Implémentation création de profils.</t>
+  </si>
+  <si>
+    <t>Implémentation création de profils.</t>
+  </si>
+  <si>
+    <t>Création UI gestion de profils.</t>
+  </si>
+  <si>
+    <t>Implémentation gestion de profils.</t>
+  </si>
+  <si>
+    <t>Implémentation sélection des joueurs .</t>
+  </si>
+  <si>
+    <t>Fin Implémentation sélection des joueurs.</t>
+  </si>
+  <si>
+    <t>Création UI Sélection des joueurs.</t>
+  </si>
+  <si>
+    <t>Prototype de remplissage de grille.</t>
+  </si>
+  <si>
+    <t>Ajout des pièces sur le plateau. Considération des futures classes à ajouter.</t>
+  </si>
+  <si>
+    <t>Ajout des classes "Game" et "Joueur". De plus, les cases ont désormais un type.</t>
+  </si>
+  <si>
+    <t>Ajout des déplacements, de l'élimination des pièces et des conditions de victoire.</t>
+  </si>
+  <si>
+    <t>Ajout de l'écran de fin.</t>
+  </si>
+  <si>
+    <t>Révision du code de form_Confirmation.cs. Import des ressources.</t>
+  </si>
+  <si>
+    <t>Révision du code .</t>
+  </si>
+  <si>
+    <t>Tests de création d'un installeur dans un programme parrallèle de test et test d'ajout de musiques d'arrière plan.</t>
+  </si>
+  <si>
+    <t>Ajout musiques d'ambiance et ajout du "Setup project".</t>
+  </si>
+  <si>
+    <t>Tests.</t>
+  </si>
+  <si>
+    <t>Création d'images pour la documentation.</t>
+  </si>
+  <si>
+    <t>Diagrammes de classes.</t>
+  </si>
+  <si>
+    <t>Ajustement d'une règle d'élimination.</t>
+  </si>
+  <si>
+    <t>40 minutes</t>
+  </si>
+  <si>
+    <t>2h20</t>
+  </si>
+  <si>
+    <t>Toutes les pages ont été relues.</t>
+  </si>
+  <si>
+    <t>Gestion de profils fonctionnelle avec messages d'erreurs en cas de mauvaises manipulations.</t>
+  </si>
+  <si>
+    <t>En cours, les listes déroulantes se remplissent. Il faut encore ajouter une erreur si deux même profils sont choisis</t>
+  </si>
+  <si>
+    <t>Les jouers doivent être sélectionnés pour lancer une partie. Doublon impossible.</t>
+  </si>
+  <si>
+    <t>Un table layout panel a été placé au dessus du dessin du plateau, de ce fait il sera possible de placer les pions en fonctions d'une ligne et d'une colonne.</t>
+  </si>
+  <si>
+    <t>Une classe Square, héritée de picture box a été créée. Elle inclut une énumération personnalisée.</t>
+  </si>
+  <si>
+    <t>Le formulaire de "Game_Error" a été retiré, le jeu est désormais fonctionnel. Il ne reste qu'a revoir le code et créer un utilisateur spécial pour la base de données.</t>
+  </si>
+  <si>
+    <t>Création d'un utilisateur pour la base de donnée. Correctif du pion roi. Recherche de méthodes d'exécution du script sql pour les futurs utilisateurs. Révision du code et des commentaires.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les commentaires ont été revus, une énmération a été ajoutée pour simplifier la compréhension. </t>
+  </si>
+  <si>
+    <t>Ce formulaire permet de pouvoir observer l'état final du plateau. Les musiques d'ambiance n'ont pas encore pu être implémentées.</t>
+  </si>
+  <si>
+    <t>L'installeur installe toutes les dépendances. Reste à ajouter les modifications sur le projet de base.</t>
+  </si>
+  <si>
+    <t>Les tests sont terminés, rien à signaler.</t>
+  </si>
+  <si>
+    <t>Plusieurs diagrammes sont créés pour dais raison de mise en page.</t>
+  </si>
+  <si>
+    <t>Images des diagrammes de classe et des maquettes.</t>
+  </si>
+  <si>
+    <t>Le roi ne pouvait pas être éliminé si adjacent au trone. Pourtant il est expliqué explicitement qu'il est possible. Cependant les règles sont approximatives, il y a donc des moyens pour ne pas être éliminé (laisser un pion dans un coin p.ex.).</t>
+  </si>
+  <si>
+    <t>Certaines fenêtres pouvaient être agrandies alors que non. Ajout d'un try catch sur une zone de mise à jour de la base de données. Ajout des sons sur le bouton du volume. Création d'un dossier rendu. Correctif, le roi peut s'auto-éliminer. Relecture de la documentation.</t>
+  </si>
+  <si>
+    <t>Relecture des commentaires du code.</t>
+  </si>
+  <si>
+    <t>Rechargement de la documentation effectuée.</t>
+  </si>
+  <si>
+    <t>Ajustements et vérifications.</t>
+  </si>
+  <si>
+    <t>Tous les fichiers qui doivent être rendus sont présents.</t>
   </si>
 </sst>
 </file>
@@ -588,7 +600,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -637,6 +649,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -972,10 +987,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G72"/>
+  <dimension ref="B1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57:G57"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I59" sqref="I59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -989,22 +1004,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
     </row>
     <row r="2" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
     </row>
     <row r="3" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
@@ -1015,18 +1030,18 @@
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="33"/>
+      <c r="C4" s="34"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="2:7" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -1043,11 +1058,11 @@
       <c r="D7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="34" t="s">
+      <c r="E7" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
     </row>
     <row r="8" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
@@ -1059,11 +1074,11 @@
       <c r="D8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="27"/>
-      <c r="G8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="29"/>
     </row>
     <row r="9" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
@@ -1075,9 +1090,9 @@
       <c r="D9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="25"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="26"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="4">
@@ -1103,9 +1118,9 @@
       <c r="D11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="25"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="26"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
@@ -1145,9 +1160,9 @@
       <c r="D14" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="29"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="31"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="32"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
@@ -1159,9 +1174,9 @@
       <c r="D15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="23"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="25"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="26"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="4">
@@ -1173,9 +1188,9 @@
       <c r="D16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="23"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="25"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="26"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="4">
@@ -1201,9 +1216,9 @@
       <c r="D18" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="23"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="25"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="26"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="4">
@@ -1215,9 +1230,9 @@
       <c r="D19" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="23"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="25"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="26"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="4">
@@ -1229,11 +1244,11 @@
       <c r="D20" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="23" t="s">
+      <c r="E20" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="F20" s="24"/>
-      <c r="G20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="26"/>
     </row>
     <row r="21" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B21" s="4">
@@ -1245,9 +1260,9 @@
       <c r="D21" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="23"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="25"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="26"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="4">
@@ -1259,9 +1274,9 @@
       <c r="D22" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="23"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="25"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="26"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="4">
@@ -1273,664 +1288,575 @@
       <c r="D23" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="23"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="25"/>
-    </row>
-    <row r="24" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E23" s="24"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="26"/>
+    </row>
+    <row r="24" spans="2:7" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="4">
         <v>43146</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="29" t="s">
+      <c r="E24" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="F24" s="30"/>
-      <c r="G24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="32"/>
     </row>
     <row r="25" spans="2:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="4">
         <v>43147</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E25" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="F25" s="30"/>
-      <c r="G25" s="31"/>
+      <c r="E25" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" s="31"/>
+      <c r="G25" s="32"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="4">
         <v>43147</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="23"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="25"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="26"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="4">
         <v>43157</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="F27" s="24"/>
-      <c r="G27" s="25"/>
+      <c r="E27" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="F27" s="25"/>
+      <c r="G27" s="26"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="4">
         <v>43158</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E28" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="F28" s="24"/>
-      <c r="G28" s="25"/>
+      <c r="E28" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28" s="25"/>
+      <c r="G28" s="26"/>
     </row>
     <row r="29" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="4">
         <v>43160</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="F29" s="30"/>
-      <c r="G29" s="31"/>
+      <c r="E29" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="F29" s="31"/>
+      <c r="G29" s="32"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="4">
         <v>43160</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E30" s="23"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="25"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="26"/>
     </row>
     <row r="31" spans="2:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="4">
         <v>43160</v>
       </c>
-      <c r="C31" s="10" t="s">
-        <v>41</v>
+      <c r="C31" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="F31" s="30"/>
-      <c r="G31" s="31"/>
+      <c r="E31" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="F31" s="31"/>
+      <c r="G31" s="32"/>
     </row>
     <row r="32" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="4">
         <v>43161</v>
       </c>
-      <c r="C32" s="10" t="s">
-        <v>43</v>
+      <c r="C32" s="9" t="s">
+        <v>56</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E32" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="F32" s="30"/>
-      <c r="G32" s="31"/>
+      <c r="E32" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="F32" s="31"/>
+      <c r="G32" s="32"/>
     </row>
     <row r="33" spans="2:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="4">
         <v>43161</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="F33" s="30"/>
-      <c r="G33" s="31"/>
+      <c r="E33" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="F33" s="31"/>
+      <c r="G33" s="32"/>
     </row>
     <row r="34" spans="2:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="15">
         <v>43164</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E34" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="F34" s="30"/>
-      <c r="G34" s="31"/>
+      <c r="E34" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="F34" s="31"/>
+      <c r="G34" s="32"/>
     </row>
     <row r="35" spans="2:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B35" s="4">
         <v>43165</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E35" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="F35" s="30"/>
-      <c r="G35" s="31"/>
+      <c r="E35" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="F35" s="31"/>
+      <c r="G35" s="32"/>
     </row>
     <row r="36" spans="2:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B36" s="4">
         <v>43167</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E36" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="F36" s="30"/>
-      <c r="G36" s="31"/>
+        <v>36</v>
+      </c>
+      <c r="E36" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F36" s="31"/>
+      <c r="G36" s="32"/>
     </row>
     <row r="37" spans="2:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="4">
         <v>43168</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E37" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="F37" s="30"/>
-      <c r="G37" s="31"/>
+      <c r="E37" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="F37" s="31"/>
+      <c r="G37" s="32"/>
     </row>
     <row r="38" spans="2:7" ht="110.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="4">
         <v>43171</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E38" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="F38" s="30"/>
-      <c r="G38" s="31"/>
+      <c r="E38" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="F38" s="31"/>
+      <c r="G38" s="32"/>
     </row>
     <row r="39" spans="2:7" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B39" s="4">
         <v>43172</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E39" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="F39" s="30"/>
-      <c r="G39" s="31"/>
-    </row>
-    <row r="40" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E39" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="F39" s="31"/>
+      <c r="G39" s="32"/>
+    </row>
+    <row r="40" spans="2:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="4">
         <v>43174</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E40" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="F40" s="30"/>
-      <c r="G40" s="31"/>
+        <v>40</v>
+      </c>
+      <c r="E40" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="F40" s="31"/>
+      <c r="G40" s="32"/>
     </row>
     <row r="41" spans="2:7" ht="63" x14ac:dyDescent="0.25">
       <c r="B41" s="4">
         <v>43174</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E41" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="F41" s="30"/>
-      <c r="G41" s="31"/>
+        <v>41</v>
+      </c>
+      <c r="E41" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="F41" s="31"/>
+      <c r="G41" s="32"/>
     </row>
     <row r="42" spans="2:7" ht="63" x14ac:dyDescent="0.25">
       <c r="B42" s="4">
         <v>43175</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E42" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="F42" s="30"/>
-      <c r="G42" s="31"/>
+      <c r="E42" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="F42" s="31"/>
+      <c r="G42" s="32"/>
     </row>
     <row r="43" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B43" s="4">
         <v>43178</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E43" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="F43" s="30"/>
-      <c r="G43" s="31"/>
+      <c r="E43" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="F43" s="31"/>
+      <c r="G43" s="32"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" s="4">
         <v>43179</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E44" s="23"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="25"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="25"/>
+      <c r="G44" s="26"/>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" s="4">
         <v>43181</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E45" s="23"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="25"/>
+        <v>36</v>
+      </c>
+      <c r="E45" s="24"/>
+      <c r="F45" s="25"/>
+      <c r="G45" s="26"/>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" s="4">
         <v>43182</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E46" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="F46" s="24"/>
-      <c r="G46" s="25"/>
+      <c r="E46" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="F46" s="25"/>
+      <c r="G46" s="26"/>
     </row>
     <row r="47" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B47" s="4">
         <v>43185</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E47" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="F47" s="30"/>
-      <c r="G47" s="31"/>
+      <c r="E47" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="F47" s="31"/>
+      <c r="G47" s="32"/>
     </row>
     <row r="48" spans="2:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="4">
         <v>43186</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E48" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="F48" s="30"/>
-      <c r="G48" s="31"/>
+      <c r="E48" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="F48" s="31"/>
+      <c r="G48" s="32"/>
     </row>
     <row r="49" spans="2:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B49" s="4">
         <v>43188</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E49" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="F49" s="24"/>
-      <c r="G49" s="25"/>
+      <c r="E49" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="F49" s="31"/>
+      <c r="G49" s="32"/>
     </row>
     <row r="50" spans="2:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="4">
         <v>43188</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E50" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="F50" s="30"/>
-      <c r="G50" s="31"/>
-    </row>
-    <row r="51" spans="2:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="4">
+        <v>71</v>
+      </c>
+      <c r="E50" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="F50" s="31"/>
+      <c r="G50" s="32"/>
+    </row>
+    <row r="51" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="16">
         <v>43188</v>
       </c>
-      <c r="C51" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E51" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="F51" s="30"/>
-      <c r="G51" s="31"/>
+      <c r="C51" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E51" s="18"/>
+      <c r="F51" s="19"/>
+      <c r="G51" s="20"/>
     </row>
     <row r="52" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="16">
-        <v>43188</v>
+        <v>43201</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E52" s="17"/>
-      <c r="F52" s="18"/>
-      <c r="G52" s="19"/>
+        <v>46</v>
+      </c>
+      <c r="E52" s="18"/>
+      <c r="F52" s="19"/>
+      <c r="G52" s="20"/>
     </row>
     <row r="53" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B53" s="16">
-        <v>43201</v>
+        <v>43202</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E53" s="17"/>
-      <c r="F53" s="18"/>
-      <c r="G53" s="19"/>
+        <v>46</v>
+      </c>
+      <c r="E53" s="18"/>
+      <c r="F53" s="19"/>
+      <c r="G53" s="20"/>
     </row>
     <row r="54" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="16">
-        <v>43202</v>
+        <v>43203</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E54" s="17"/>
-      <c r="F54" s="18"/>
-      <c r="G54" s="19"/>
-    </row>
-    <row r="55" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="E54" s="18"/>
+      <c r="F54" s="19"/>
+      <c r="G54" s="20"/>
+    </row>
+    <row r="55" spans="2:7" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="16">
-        <v>43203</v>
+        <v>43206</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>85</v>
+        <v>48</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E55" s="17"/>
-      <c r="F55" s="18"/>
-      <c r="G55" s="19"/>
-    </row>
-    <row r="56" spans="2:7" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="E55" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="F55" s="22"/>
+      <c r="G55" s="23"/>
+    </row>
+    <row r="56" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="16">
-        <v>43206</v>
+        <v>43207</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>86</v>
+        <v>49</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E56" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="F56" s="21"/>
-      <c r="G56" s="22"/>
+      <c r="E56" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F56" s="19"/>
+      <c r="G56" s="20"/>
     </row>
     <row r="57" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="16">
-        <v>43207</v>
+        <v>43209</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>88</v>
+        <v>49</v>
       </c>
       <c r="D57" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E57" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="F57" s="19"/>
+      <c r="G57" s="20"/>
+    </row>
+    <row r="58" spans="2:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="16">
+        <v>43209</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D58" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E57" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="F57" s="18"/>
-      <c r="G57" s="19"/>
-    </row>
-    <row r="58" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="16"/>
-      <c r="C58" s="11"/>
-      <c r="D58" s="6"/>
-      <c r="E58" s="17"/>
-      <c r="F58" s="18"/>
-      <c r="G58" s="19"/>
-    </row>
-    <row r="59" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="16"/>
-      <c r="C59" s="11"/>
-      <c r="D59" s="6"/>
-      <c r="E59" s="17"/>
-      <c r="F59" s="18"/>
-      <c r="G59" s="19"/>
-    </row>
-    <row r="60" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="16"/>
-      <c r="C60" s="11"/>
-      <c r="D60" s="6"/>
-      <c r="E60" s="17"/>
-      <c r="F60" s="18"/>
-      <c r="G60" s="19"/>
-    </row>
-    <row r="61" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="16"/>
-      <c r="C61" s="11"/>
-      <c r="D61" s="6"/>
-      <c r="E61" s="17"/>
-      <c r="F61" s="18"/>
-      <c r="G61" s="19"/>
-    </row>
-    <row r="62" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="16"/>
-      <c r="C62" s="11"/>
-      <c r="D62" s="6"/>
-      <c r="E62" s="17"/>
-      <c r="F62" s="18"/>
-      <c r="G62" s="19"/>
-    </row>
-    <row r="63" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="16"/>
-      <c r="C63" s="11"/>
-      <c r="D63" s="6"/>
-      <c r="E63" s="17"/>
-      <c r="F63" s="18"/>
-      <c r="G63" s="19"/>
-    </row>
-    <row r="64" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="16"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="6"/>
-      <c r="E64" s="17"/>
-      <c r="F64" s="18"/>
-      <c r="G64" s="19"/>
-    </row>
-    <row r="65" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="16"/>
-      <c r="C65" s="11"/>
-      <c r="D65" s="6"/>
-      <c r="E65" s="17"/>
-      <c r="F65" s="18"/>
-      <c r="G65" s="19"/>
-    </row>
-    <row r="66" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="16"/>
-      <c r="C66" s="11"/>
-      <c r="D66" s="6"/>
-      <c r="E66" s="17"/>
-      <c r="F66" s="18"/>
-      <c r="G66" s="19"/>
-    </row>
-    <row r="67" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="16"/>
-      <c r="C67" s="11"/>
-      <c r="D67" s="6"/>
-      <c r="E67" s="17"/>
-      <c r="F67" s="18"/>
-      <c r="G67" s="19"/>
-    </row>
-    <row r="68" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="16"/>
-      <c r="C68" s="11"/>
-      <c r="D68" s="6"/>
-      <c r="E68" s="17"/>
-      <c r="F68" s="18"/>
-      <c r="G68" s="19"/>
-    </row>
-    <row r="69" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="16"/>
-      <c r="C69" s="11"/>
-      <c r="D69" s="6"/>
-      <c r="E69" s="17"/>
-      <c r="F69" s="18"/>
-      <c r="G69" s="19"/>
-    </row>
-    <row r="70" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="16"/>
-      <c r="C70" s="11"/>
-      <c r="D70" s="6"/>
-      <c r="E70" s="17"/>
-      <c r="F70" s="18"/>
-      <c r="G70" s="19"/>
-    </row>
-    <row r="71" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="16"/>
-      <c r="C71" s="11"/>
-      <c r="D71" s="6"/>
-      <c r="E71" s="17"/>
-      <c r="F71" s="18"/>
-      <c r="G71" s="19"/>
-    </row>
-    <row r="72" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="16"/>
-      <c r="C72" s="11"/>
-      <c r="D72" s="6"/>
-      <c r="E72" s="17"/>
-      <c r="F72" s="18"/>
-      <c r="G72" s="19"/>
+      <c r="E58" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="F58" s="19"/>
+      <c r="G58" s="20"/>
+    </row>
+    <row r="59" spans="2:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="16">
+        <v>43270</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E59" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="F59" s="22"/>
+      <c r="G59" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="64">
+  <mergeCells count="51">
     <mergeCell ref="E49:G49"/>
     <mergeCell ref="E50:G50"/>
     <mergeCell ref="E51:G51"/>
-    <mergeCell ref="E52:G52"/>
     <mergeCell ref="E43:G43"/>
     <mergeCell ref="E44:G44"/>
     <mergeCell ref="E45:G45"/>
@@ -1971,29 +1897,17 @@
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="E58:G58"/>
+    <mergeCell ref="E59:G59"/>
+    <mergeCell ref="E52:G52"/>
     <mergeCell ref="E53:G53"/>
     <mergeCell ref="E54:G54"/>
     <mergeCell ref="E55:G55"/>
     <mergeCell ref="E56:G56"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="E58:G58"/>
-    <mergeCell ref="E59:G59"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="E61:G61"/>
-    <mergeCell ref="E62:G62"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="E64:G64"/>
-    <mergeCell ref="E65:G65"/>
-    <mergeCell ref="E66:G66"/>
-    <mergeCell ref="E67:G67"/>
-    <mergeCell ref="E68:G68"/>
-    <mergeCell ref="E69:G69"/>
-    <mergeCell ref="E70:G70"/>
-    <mergeCell ref="E71:G71"/>
-    <mergeCell ref="E72:G72"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="74" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>